<commit_message>
some BG test results
</commit_message>
<xml_diff>
--- a/TestResult/update_read_staleness.xlsx
+++ b/TestResult/update_read_staleness.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="3280" windowWidth="25600" windowHeight="14000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -103,6 +103,298 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>工作表1!$A$13:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4165.63117692803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3311.71318190901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3029.47788409339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2769.22910401284</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2575.1760566312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2115.54191547963</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2021.25994348222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1898.17324985012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1759.76113994727</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1659.81656081501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>工作表1!$A$13:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$D$13:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3775.20815293412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3255.3049768451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2735.35058840769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2362.43528536054</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2195.42729634316</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2036.89296460906</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007.17541209912</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1743.92441192437</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1751.9487245242</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1546.21918706985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2142741272"/>
+        <c:axId val="2142743320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2142741272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142743320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2142743320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142741272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -438,8 +730,10 @@
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -664,9 +958,166 @@
         <v>2.5624957077123801E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <f>1-2*A13</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>3775.2081529341199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <f>A13+0.05</f>
+        <v>0.05</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B22" si="2">1-2*A14</f>
+        <v>0.9</v>
+      </c>
+      <c r="D14">
+        <v>3255.3049768451001</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <f t="shared" ref="A15:A22" si="3">A14+0.05</f>
+        <v>0.1</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>2735.3505884076899</v>
+      </c>
+      <c r="H15">
+        <v>0.12198232417466499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="D16">
+        <v>2362.4352853605401</v>
+      </c>
+      <c r="H16">
+        <v>0.14388968686078599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="D17">
+        <v>2195.4272963431599</v>
+      </c>
+      <c r="H17">
+        <v>0.127352801538759</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>2036.8929646090601</v>
+      </c>
+      <c r="H18">
+        <v>0.10244810637547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="D19">
+        <v>2007.17541209912</v>
+      </c>
+      <c r="H19">
+        <v>7.5934252884627795E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D20">
+        <v>1743.9244119243699</v>
+      </c>
+      <c r="H20">
+        <v>6.0406211335548299E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>0.20000000000000007</v>
+      </c>
+      <c r="D21">
+        <v>1751.9487245242001</v>
+      </c>
+      <c r="H21">
+        <v>4.00967074395066E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="D22">
+        <v>1546.21918706985</v>
+      </c>
+      <c r="H22">
+        <v>2.7532108674114E-2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>